<commit_message>
Added Suspended & Withdrawn FTs and some minor update
</commit_message>
<xml_diff>
--- a/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
+++ b/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UKHO - ERP Facade\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prash1501461\Source\Repos\UKHO\erp-facade\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
   <si>
     <t>ID#</t>
   </si>
@@ -258,6 +258,120 @@
   </si>
   <si>
     <t>Cancel &amp; replace + metadata change + move cell</t>
+  </si>
+  <si>
+    <t>ID20</t>
+  </si>
+  <si>
+    <t>ID21</t>
+  </si>
+  <si>
+    <t>ID22</t>
+  </si>
+  <si>
+    <t>ID23</t>
+  </si>
+  <si>
+    <t>ID24</t>
+  </si>
+  <si>
+    <t>ID25</t>
+  </si>
+  <si>
+    <t>ID26</t>
+  </si>
+  <si>
+    <t>ID27</t>
+  </si>
+  <si>
+    <t>ID28</t>
+  </si>
+  <si>
+    <t>ID29</t>
+  </si>
+  <si>
+    <t>ID30</t>
+  </si>
+  <si>
+    <t>ID31</t>
+  </si>
+  <si>
+    <t>ID32</t>
+  </si>
+  <si>
+    <t>New Edition additional coverage v0.1</t>
+  </si>
+  <si>
+    <t>cancelAndReplaceV03</t>
+  </si>
+  <si>
+    <t>Cell_Moves_Unit_and_New_CellV03</t>
+  </si>
+  <si>
+    <t>Cell_MoveV03</t>
+  </si>
+  <si>
+    <t>Metadata_ChangeV03</t>
+  </si>
+  <si>
+    <t>Mixed_scenario1V03</t>
+  </si>
+  <si>
+    <t>New_CellV03</t>
+  </si>
+  <si>
+    <t>supplier_Defined_ReleasabilitySet_V01</t>
+  </si>
+  <si>
+    <t>simpleSuspendedScenario</t>
+  </si>
+  <si>
+    <t>simpleWithdrawnScenario</t>
+  </si>
+  <si>
+    <t>Suspend_and_WithdrawV01</t>
+  </si>
+  <si>
+    <t>metadataAndSuspended</t>
+  </si>
+  <si>
+    <t>moveAndSuspended</t>
+  </si>
+  <si>
+    <t>Move Cell + Suspended</t>
+  </si>
+  <si>
+    <t>Metadata Change + Suspended</t>
+  </si>
+  <si>
+    <t>Suspended + Withdrawn</t>
+  </si>
+  <si>
+    <t>Simple Suspended</t>
+  </si>
+  <si>
+    <t>Simple Withdrawn</t>
+  </si>
+  <si>
+    <t>New Cell V0.3</t>
+  </si>
+  <si>
+    <t>Metadata Change V0.3</t>
+  </si>
+  <si>
+    <t>Move Cell V0.3</t>
+  </si>
+  <si>
+    <t>Move Cell + New Cell V0.3</t>
+  </si>
+  <si>
+    <t>Cancel &amp; Replace V0.3</t>
+  </si>
+  <si>
+    <t>Mix Scenario V0.1</t>
+  </si>
+  <si>
+    <t>Mix Scenario V0.3</t>
   </si>
 </sst>
 </file>
@@ -328,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -352,11 +466,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -640,9 +764,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -733,7 +860,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="4" t="str">
-        <f t="shared" ref="C5:C20" si="0">CONCATENATE(A5,"_",B5)</f>
+        <f t="shared" ref="C5:C33" si="0">CONCATENATE(A5,"_",B5)</f>
         <v>ID4_2NewCellScenario.JSON</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1009,9 +1136,217 @@
         <v>69</v>
       </c>
     </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID20_New Edition additional coverage v0.1</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID21_cancelAndReplaceV03</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID22_Cell_Moves_Unit_and_New_CellV03</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID23_Cell_MoveV03</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID24_Metadata_ChangeV03</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID25_Mixed_scenario1V03</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID26_New_CellV03</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID27_supplier_Defined_ReleasabilitySet_V01</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID28_simpleSuspendedScenario</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID29_simpleWithdrawnScenario</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID30_Suspend_and_WithdrawV01</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID31_metadataAndSuspended</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID32_moveAndSuspended</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:E20">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A2:E33">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update Scenario Mapping excel file
</commit_message>
<xml_diff>
--- a/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
+++ b/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="122">
   <si>
     <t>ID#</t>
   </si>
@@ -372,6 +372,86 @@
   </si>
   <si>
     <t>Mix Scenario V0.3</t>
+  </si>
+  <si>
+    <t>"contentChanged": false,
+"statusName": "Suspended",</t>
+  </si>
+  <si>
+    <t>"contentChanged": false,
+"statusName": "Suspended",
+WHEN EXIST addProduct items  AND
+WHEN EXIST removeProduct item AND</t>
+  </si>
+  <si>
+    <t>Cell1:
+"contentChanged": false,
+"statusName": "Withdrawn",
+Cell2:
+"contentChanged": false
+"statusName": Suspended 
+-------------------------------------
+WHEN EXIST addProduct items  AND
+WHEN EXIST removeProduct item AND</t>
+  </si>
+  <si>
+    <t>"contentChanged": true,
+"statusName": "Withdrawn",
+WHEN EXIST addProduct items  AND
+WHEN EXIST removeProduct item AND
+CANCEL AVCS UOS WHEN STATUS="NotForSale"</t>
+  </si>
+  <si>
+    <t>"contentChanged": true,
+"statusName": "Suspended",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"contentChange": true,
+"statusName": "Update",
+</t>
+  </si>
+  <si>
+    <t>"contentChanged": true,
+"isNewCell": true,</t>
+  </si>
+  <si>
+    <t>isNewCell = true &amp; IsNewUnitOfSale = true
+WHEN StatusName = “New Edition” AND
+WHEN EXIST addProduct items  AND
+WHEN EXIST removeProduct item AND</t>
+  </si>
+  <si>
+    <t>contentChanged = false</t>
+  </si>
+  <si>
+    <t>If “contentChanged”:false
+WHEN EXIST addProduct items  AND
+WHEN EXIST removeProduct item AND</t>
+  </si>
+  <si>
+    <t>If “contentChanged”:false
+isNewCell=true,
+inUnitOfSales contains multiple unit of sales with unitOfSaleType="unit",
+WHEN EXIST addProduct items  AND
+WHEN EXIST removeProduct item AND</t>
+  </si>
+  <si>
+    <t>"contentChanged": true,
+"statusName": "New Edition",
+"isNewCell": false,</t>
+  </si>
+  <si>
+    <t>"contentChanged": true,
+WHEN EXIST addProduct items  AND
+WHEN EXIST replacedBy items AND
+WHEN EXIST removeProduct item AND</t>
+  </si>
+  <si>
+    <t>"contentChanged": true,
+"statusName": "New Edition",
+WHEN EXIST addProduct items  AND
+WHEN EXIST replacedBy items AND
+WHEN EXIST removeProduct item AND</t>
   </si>
 </sst>
 </file>
@@ -473,14 +553,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -766,9 +839,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,7 +1177,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>64</v>
       </c>
@@ -1115,12 +1188,14 @@
         <f t="shared" si="0"/>
         <v>ID18_ID18_CancelReplace_UpdateCell.JSON</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="E19" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>67</v>
       </c>
@@ -1131,12 +1206,14 @@
         <f t="shared" si="0"/>
         <v>ID19_ID19_CR_metadata_move.JSON</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>120</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
@@ -1147,12 +1224,14 @@
         <f t="shared" si="0"/>
         <v>ID20_New Edition additional coverage v0.1</v>
       </c>
-      <c r="D21" s="9"/>
+      <c r="D21" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="E21" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>71</v>
       </c>
@@ -1163,12 +1242,14 @@
         <f t="shared" si="0"/>
         <v>ID21_cancelAndReplaceV03</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="E22" s="9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>72</v>
       </c>
@@ -1179,12 +1260,14 @@
         <f t="shared" si="0"/>
         <v>ID22_Cell_Moves_Unit_and_New_CellV03</v>
       </c>
-      <c r="D23" s="9"/>
+      <c r="D23" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="E23" s="9" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -1195,7 +1278,9 @@
         <f t="shared" si="0"/>
         <v>ID23_Cell_MoveV03</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="E24" s="9" t="s">
         <v>103</v>
       </c>
@@ -1211,12 +1296,14 @@
         <f t="shared" si="0"/>
         <v>ID24_Metadata_ChangeV03</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="E25" s="9" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>75</v>
       </c>
@@ -1227,12 +1314,14 @@
         <f t="shared" si="0"/>
         <v>ID25_Mixed_scenario1V03</v>
       </c>
-      <c r="D26" s="9"/>
+      <c r="D26" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="E26" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>76</v>
       </c>
@@ -1243,12 +1332,14 @@
         <f t="shared" si="0"/>
         <v>ID26_New_CellV03</v>
       </c>
-      <c r="D27" s="9"/>
+      <c r="D27" s="5" t="s">
+        <v>114</v>
+      </c>
       <c r="E27" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
@@ -1259,12 +1350,14 @@
         <f t="shared" si="0"/>
         <v>ID27_supplier_Defined_ReleasabilitySet_V01</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="E28" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>78</v>
       </c>
@@ -1275,12 +1368,14 @@
         <f t="shared" si="0"/>
         <v>ID28_simpleSuspendedScenario</v>
       </c>
-      <c r="D29" s="9"/>
+      <c r="D29" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="E29" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>79</v>
       </c>
@@ -1291,12 +1386,14 @@
         <f t="shared" si="0"/>
         <v>ID29_simpleWithdrawnScenario</v>
       </c>
-      <c r="D30" s="9"/>
+      <c r="D30" s="5" t="s">
+        <v>111</v>
+      </c>
       <c r="E30" s="9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>80</v>
       </c>
@@ -1307,12 +1404,14 @@
         <f t="shared" si="0"/>
         <v>ID30_Suspend_and_WithdrawV01</v>
       </c>
-      <c r="D31" s="9"/>
+      <c r="D31" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="E31" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>81</v>
       </c>
@@ -1323,12 +1422,14 @@
         <f t="shared" si="0"/>
         <v>ID31_metadataAndSuspended</v>
       </c>
-      <c r="D32" s="9"/>
+      <c r="D32" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="E32" s="9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>82</v>
       </c>
@@ -1339,14 +1440,16 @@
         <f t="shared" si="0"/>
         <v>ID32_moveAndSuspended</v>
       </c>
-      <c r="D33" s="9"/>
+      <c r="D33" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="E33" s="9" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:E33">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed review comments AB#83728
</commit_message>
<xml_diff>
--- a/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
+++ b/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Scenario Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="135">
   <si>
     <t>ID#</t>
   </si>
@@ -195,9 +196,6 @@
     <t>ID14_moveOneCell.JSON</t>
   </si>
   <si>
-    <t>If “contentChanged”:false</t>
-  </si>
-  <si>
     <t>Move cell</t>
   </si>
   <si>
@@ -338,9 +336,6 @@
     <t>moveAndSuspended</t>
   </si>
   <si>
-    <t>Move Cell + Suspended</t>
-  </si>
-  <si>
     <t>Metadata Change + Suspended</t>
   </si>
   <si>
@@ -376,12 +371,6 @@
   <si>
     <t>"contentChanged": false,
 "statusName": "Suspended",</t>
-  </si>
-  <si>
-    <t>"contentChanged": false,
-"statusName": "Suspended",
-WHEN EXIST addProduct items  AND
-WHEN EXIST removeProduct item AND</t>
   </si>
   <si>
     <t>Cell1:
@@ -452,6 +441,59 @@
 WHEN EXIST addProduct items  AND
 WHEN EXIST replacedBy items AND
 WHEN EXIST removeProduct item AND</t>
+  </si>
+  <si>
+    <t>ID33</t>
+  </si>
+  <si>
+    <t>ID34</t>
+  </si>
+  <si>
+    <t>ID35</t>
+  </si>
+  <si>
+    <t>ID36</t>
+  </si>
+  <si>
+    <t>NewCell_With2UoS_But_only1_having_addProduct</t>
+  </si>
+  <si>
+    <t>Cancel&amp;Replace_With_NewCells_having_2UoS_With_addProductValue</t>
+  </si>
+  <si>
+    <t>Cancel&amp;Replace_With_CancelCell_having_2UoS_but_onlyOneAsTypeUnit</t>
+  </si>
+  <si>
+    <t>MoveAndSuspended_With_2UoS_But1_Having_addProductsValue</t>
+  </si>
+  <si>
+    <t>Move + Suspended with multiple unit of sales with unitOfSalesType=unit</t>
+  </si>
+  <si>
+    <t>Cancel Replace With Cancelled Cell having 2UoS but only One As unitOfSalesType=unit</t>
+  </si>
+  <si>
+    <t>Cancel &amp; Replace With New Cells having 2 UoS both having   unitOfSalesType=unit and value in addProducts</t>
+  </si>
+  <si>
+    <t>NewCell With 2 UoS but only 1 having value in addProduct</t>
+  </si>
+  <si>
+    <t>Move and Suspended</t>
+  </si>
+  <si>
+    <t>If “contentChanged”:false
+addProducts has value
+removeProducts has value</t>
+  </si>
+  <si>
+    <t>If “contentChanged”:false
+addProducts has value
+removeProducts has value
+Status = 'Suspended'</t>
+  </si>
+  <si>
+    <t>isNewCell = true</t>
   </si>
 </sst>
 </file>
@@ -837,11 +879,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,7 +1147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
@@ -1117,54 +1159,54 @@
         <v>ID14_ID14_moveOneCell.JSON</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ID15_ID15_oneNewCellAndOneMoveOneCell.JSON</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ID15_ID15_oneNewCellAndOneMoveOneCell.JSON</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ID16_ID16_newCell_updateCell_metadataChange.JSON</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ID16_ID16_newCell_updateCell_metadataChange.JSON</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1174,69 +1216,69 @@
         <v>23</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ID18_ID18_CancelReplace_UpdateCell.JSON</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C19" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ID18_ID18_CancelReplace_UpdateCell.JSON</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ID19_ID19_CR_metadata_move.JSON</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ID19_ID19_CR_metadata_move.JSON</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID20_New Edition additional coverage v0.1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1246,209 +1288,281 @@
         <v>23</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID22_Cell_Moves_Unit_and_New_CellV03</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID23_Cell_MoveV03</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID24_Metadata_ChangeV03</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID25_Mixed_scenario1V03</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID26_New_CellV03</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID27_supplier_Defined_ReleasabilitySet_V01</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID28_simpleSuspendedScenario</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C30" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID29_simpleWithdrawnScenario</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID30_Suspend_and_WithdrawV01</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID31_metadataAndSuspended</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID32_moveAndSuspended</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>109</v>
+      <c r="D33" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>96</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" s="5" t="str">
+        <f t="shared" ref="C34:C37" si="1">CONCATENATE(A34,"_",B34)</f>
+        <v>ID33_NewCell_With2UoS_But_only1_having_addProduct</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>ID34_Cancel&amp;Replace_With_NewCells_having_2UoS_With_addProductValue</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>ID35_Cancel&amp;Replace_With_CancelCell_having_2UoS_but_onlyOneAsTypeUnit</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>ID36_MoveAndSuspended_With_2UoS_But1_Having_addProductsValue</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:E33">
+  <conditionalFormatting sqref="A2:E37">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Removed webhook 500 error testcase, uncomment line in yml file, updated scenario mapping file AB#83728
</commit_message>
<xml_diff>
--- a/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
+++ b/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prash1501461\Source\Repos\UKHO\erp-facade\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prash1501461\source\repos\UKHO\erp-facade\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Scenario Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -882,8 +881,8 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
85564 rule update for create avcs uos action (#59)
* 85564-create avcs uos rule updated for enc cell fields agency and provider

* 85564 updated logs message format AB#85564 AB#85841

* Added FTs AB#85564

* 85564-xml formating fix AB#85564 AB#86351

* 85564-code review comment fixed AB#85564

* Updated code for failing FTs AB#85564

---------

Co-authored-by: Nadeem Badai <Nadeem14456@Mastek.Com>
Co-authored-by: Prashant Gupta <prash1501461@mastek.com>
Co-authored-by: Vishal14583 <61726015+Vishal14583@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
+++ b/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prash1501461\source\repos\UKHO\erp-facade\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prash1501461\Source\Repos\UKHO\erp-facade\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="139">
   <si>
     <t>ID#</t>
   </si>
@@ -494,12 +494,51 @@
   <si>
     <t>isNewCell = true</t>
   </si>
+  <si>
+    <t>ID37</t>
+  </si>
+  <si>
+    <t>CreateUoSHavingMultipleItemsInAddProducts</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If “contentChanged”:false
+isNewCell=true,
+inUnitOfSales contains multiple unit of sales with unitOfSaleType="unit",
+WHEN EXIST </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>multiple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> addProduct items  AND
+WHEN EXIST removeProduct item AND</t>
+    </r>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMoveAndNewCellScenarioWhereUoSHasMultipleValuesInAddProducts_ThenWebhookReturns200Response</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,6 +550,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -594,7 +641,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -878,11 +939,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,7 +952,7 @@
     <col min="2" max="2" width="44.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="45.28515625" style="7" customWidth="1"/>
     <col min="4" max="4" width="55.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.5703125" style="8" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -1560,12 +1621,41 @@
         <v>127</v>
       </c>
     </row>
+    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="5" t="str">
+        <f t="shared" ref="C38" si="2">CONCATENATE(A38,"_",B38)</f>
+        <v>ID37_CreateUoSHavingMultipleItemsInAddProducts</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:E37">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:C38 E38">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ScenarioMapping file, and FT code AB#85655
</commit_message>
<xml_diff>
--- a/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
+++ b/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
@@ -12,7 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
-    <sheet name="Scenario Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Webhook Scenario Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="UnitOfSale Scenario mapping" sheetId="2" r:id="rId2"/>
+    <sheet name="PriceChange Scenario Mapping" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="216">
   <si>
     <t>ID#</t>
   </si>
@@ -69,9 +71,6 @@
   </si>
   <si>
     <t>isNewCell = true &amp; IsNewUnitOfSale = true</t>
-  </si>
-  <si>
-    <t>New Cell</t>
   </si>
   <si>
     <t>ID4</t>
@@ -104,9 +103,6 @@
 WHEN status = “NotForSale”</t>
   </si>
   <si>
-    <t>Cancel &amp; replace Cell</t>
-  </si>
-  <si>
     <t>ID7</t>
   </si>
   <si>
@@ -123,9 +119,6 @@
   </si>
   <si>
     <t>WHEN EVENT DATA contentChanged = false</t>
-  </si>
-  <si>
-    <t>Metadata Change</t>
   </si>
   <si>
     <t>ID9</t>
@@ -145,9 +138,6 @@
 StatusName =  “Update” </t>
   </si>
   <si>
-    <t>Simple Update cell</t>
-  </si>
-  <si>
     <t>ID11</t>
   </si>
   <si>
@@ -157,9 +147,6 @@
     <t>IF EVENT DATA contentChanged = true and isNewCell = false 
 AND
 StatusName =  ”New Edition”</t>
-  </si>
-  <si>
-    <t>Update cell</t>
   </si>
   <si>
     <t>ID12</t>
@@ -186,22 +173,10 @@
 StatusName =  “New Edition”</t>
   </si>
   <si>
-    <t>Multiple cell Update</t>
-  </si>
-  <si>
     <t>ID14</t>
   </si>
   <si>
-    <t>ID14_moveOneCell.JSON</t>
-  </si>
-  <si>
-    <t>Move cell</t>
-  </si>
-  <si>
     <t>ID15</t>
-  </si>
-  <si>
-    <t>ID15_oneNewCellAndOneMoveOneCell.JSON</t>
   </si>
   <si>
     <t>If “contentChanged”:false 
@@ -209,13 +184,7 @@
 isNewCell: true</t>
   </si>
   <si>
-    <t>One new cell + One move cell</t>
-  </si>
-  <si>
     <t>ID16</t>
-  </si>
-  <si>
-    <t>ID16_newCell_updateCell_metadataChange.JSON</t>
   </si>
   <si>
     <t xml:space="preserve">Cell 1: isNewCell: true
@@ -227,36 +196,15 @@
 contentChanged = false </t>
   </si>
   <si>
-    <t>new cell + update cell + metadata change</t>
-  </si>
-  <si>
     <t>ID17</t>
   </si>
   <si>
-    <t>ID17_newCell_and_CancelReplace.JSON</t>
-  </si>
-  <si>
-    <t>new cell + cancel &amp; replace</t>
-  </si>
-  <si>
     <t>ID18</t>
   </si>
   <si>
-    <t>ID18_CancelReplace_UpdateCell.JSON</t>
-  </si>
-  <si>
-    <t>Cancel &amp; replace cell + update cell</t>
-  </si>
-  <si>
     <t>ID19</t>
   </si>
   <si>
-    <t>ID19_CR_metadata_move.JSON</t>
-  </si>
-  <si>
-    <t>Cancel &amp; replace + metadata change + move cell</t>
-  </si>
-  <si>
     <t>ID20</t>
   </si>
   <si>
@@ -333,39 +281,6 @@
   </si>
   <si>
     <t>moveAndSuspended</t>
-  </si>
-  <si>
-    <t>Metadata Change + Suspended</t>
-  </si>
-  <si>
-    <t>Suspended + Withdrawn</t>
-  </si>
-  <si>
-    <t>Simple Suspended</t>
-  </si>
-  <si>
-    <t>Simple Withdrawn</t>
-  </si>
-  <si>
-    <t>New Cell V0.3</t>
-  </si>
-  <si>
-    <t>Metadata Change V0.3</t>
-  </si>
-  <si>
-    <t>Move Cell V0.3</t>
-  </si>
-  <si>
-    <t>Move Cell + New Cell V0.3</t>
-  </si>
-  <si>
-    <t>Cancel &amp; Replace V0.3</t>
-  </si>
-  <si>
-    <t>Mix Scenario V0.1</t>
-  </si>
-  <si>
-    <t>Mix Scenario V0.3</t>
   </si>
   <si>
     <t>"contentChanged": false,
@@ -464,21 +379,6 @@
   </si>
   <si>
     <t>MoveAndSuspended_With_2UoS_But1_Having_addProductsValue</t>
-  </si>
-  <si>
-    <t>Move + Suspended with multiple unit of sales with unitOfSalesType=unit</t>
-  </si>
-  <si>
-    <t>Cancel Replace With Cancelled Cell having 2UoS but only One As unitOfSalesType=unit</t>
-  </si>
-  <si>
-    <t>Cancel &amp; Replace With New Cells having 2 UoS both having   unitOfSalesType=unit and value in addProducts</t>
-  </si>
-  <si>
-    <t>NewCell With 2 UoS but only 1 having value in addProduct</t>
-  </si>
-  <si>
-    <t>Move and Suspended</t>
   </si>
   <si>
     <t>If “contentChanged”:false
@@ -532,6 +432,339 @@
   </si>
   <si>
     <t>WhenICallTheWebhookWithMoveAndNewCellScenarioWhereUoSHasMultipleValuesInAddProducts_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>Webhook Input File name</t>
+  </si>
+  <si>
+    <t>UoS input File name</t>
+  </si>
+  <si>
+    <t>WhenValidEventReceivedWithValidToken_ThenUoSReturns200OkResponse</t>
+  </si>
+  <si>
+    <t>ID1_WebhookPayload.JSON</t>
+  </si>
+  <si>
+    <t>UoS1_Pricing.JSON</t>
+  </si>
+  <si>
+    <t>UoS return 200 ok for valid payload and token</t>
+  </si>
+  <si>
+    <t>WhenValidEventReceivedWithInvalidToken_ThenUoSReturns401UnAuthorizedResponse</t>
+  </si>
+  <si>
+    <t>UoS return 401 Unauthorized for valid payload and Invalid token</t>
+  </si>
+  <si>
+    <t>WhenReceivePriceInfoForAllUoSSentToSAP_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>When Receive PriceInfo for All UoS Sent To SAP UoS Return 200Ok Response</t>
+  </si>
+  <si>
+    <t>WhenPriceInfoIsBlankFromSAP_ThenPriceSectionIsEmptyInFinalUoS_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS3_ProductMissingUOS.JSON</t>
+  </si>
+  <si>
+    <t>When PriceInfo is blank from SAP for any product then Price Section Is Empty In Final UoS</t>
+  </si>
+  <si>
+    <t>WhenPriceInfoIsNullFromSAP_ThenPriceSectionIsEmptyInFinalUoS_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS2_ProductISNullUOS.JSON</t>
+  </si>
+  <si>
+    <t>When PriceInfo is null from SAP for any product then Price Section Is Empty In Final UoS</t>
+  </si>
+  <si>
+    <t>WhenNoCorrIdinUoSrequest_UoSReturn400BadrequestResponse</t>
+  </si>
+  <si>
+    <t>When No CorrId in UoSrequest UoS Return 400Badrequest Response</t>
+  </si>
+  <si>
+    <t>WhenInvalidCorrIdinUoSrequest_UoSReturn404NotFoundResponse</t>
+  </si>
+  <si>
+    <t>When Invalid CorrId in UoSrequest UoS Return 400Badrequest Response</t>
+  </si>
+  <si>
+    <t>WhenValidCorrIdPassed_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS return 200 ok for valid payload and shared key</t>
+  </si>
+  <si>
+    <t>WhenValidCorrIdWithFutureDateBlank_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS_4_FutureDateFieldBlank.JSON</t>
+  </si>
+  <si>
+    <t>UoS return 200 ok for valid payload and Future Date Blank</t>
+  </si>
+  <si>
+    <t>WhenValidCorrIdMultiProdSameDuration_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS_5_MultiProductSameDuration.JSON</t>
+  </si>
+  <si>
+    <t>UoS return 200 ok for valid payload and same duration for multiple products</t>
+  </si>
+  <si>
+    <t>WhenValidCorrIdMultiProdMultiDuration_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS_6_MultiProductMultiDuration.JSON</t>
+  </si>
+  <si>
+    <t>UoS return 200 ok for valid payload and multiple duration for multiple products</t>
+  </si>
+  <si>
+    <t>WhenSameEffectiveAndFutureDate_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS_7_SameEffectiveSameFutureDate.JSON</t>
+  </si>
+  <si>
+    <t>UoS return 200 ok for valid payload and same Effective and Future Date</t>
+  </si>
+  <si>
+    <t>WhenDiffEffectiveAndSameFutureDate_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS_8_DiffEffectiveSameFutureDate.JSON</t>
+  </si>
+  <si>
+    <t>UoS return 200 ok for valid payload and diffrent Effective and same Future Date</t>
+  </si>
+  <si>
+    <t>WhenSameEffectiveAndDiffFutureDate_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS_9_SameEffectiveDiffFutureDate.JSON</t>
+  </si>
+  <si>
+    <t>UoS return 200 ok for valid payload and same Effective and different Future Date</t>
+  </si>
+  <si>
+    <t>WhenDiffEffectiveAndDiffFutureDate_UoSReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>UoS_10_DiffntEffectiveAndDiffFutureDate.JSON</t>
+  </si>
+  <si>
+    <t>WhenPAYSFwith12MonthDuration_UoSAlteredPAYSFPricesFinalJson</t>
+  </si>
+  <si>
+    <t>UoS_12_SAPPricing_PAYSF12Months.JSON</t>
+  </si>
+  <si>
+    <t>If SAP Price info contains PAYSF with 12 month Duration, UoS AltersPAYSF prices in final json</t>
+  </si>
+  <si>
+    <t>PriceChange Input File name</t>
+  </si>
+  <si>
+    <t>WhenValidPriceChangeEventReceivedWithValidToken_ThenPriceChangeReturns200OkResponse</t>
+  </si>
+  <si>
+    <t>PC1_MultipleProduct.JSON</t>
+  </si>
+  <si>
+    <t>PriceChange return 200 ok for valid payload and token</t>
+  </si>
+  <si>
+    <t>WhenValidPriceChangeEventReceivedWithInvalidToken_ThenPriceChangeReturns401UnAuthorizedResponse</t>
+  </si>
+  <si>
+    <t>PriceChange return 401 Unauthorized for valid payload and Invalid token</t>
+  </si>
+  <si>
+    <t>WhenMultipleProduct_ThenPriceChangeReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>PriceChange return 200 ok for valid payload and multiple products</t>
+  </si>
+  <si>
+    <t>WhenFutureDateBlank_ThenPriceChangeReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>PC2_FutureDateBlank.JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PriceChange return 200 ok for valid payload and FutureDate Field as Blank </t>
+  </si>
+  <si>
+    <t>WhenMultipleProductDifferentDuration_ThenPriceChangeReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>PC3_MultipleProductDifferentDuration.JSON</t>
+  </si>
+  <si>
+    <t>PriceChange return 200 ok for valid payload With MultipleProductDifferentDuration</t>
+  </si>
+  <si>
+    <t>WhenMultipleDurationSameEffectiveAndFutureDate_ThenPriceChangeReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>PC4_MultipleDurationSameEffectiveAndFutureDate.JSON</t>
+  </si>
+  <si>
+    <t>PriceChange return 200 ok for valid payload With MultipleDurationSameEffectiveAndFutureDate</t>
+  </si>
+  <si>
+    <t>WhenMultipleDurationDifferentEffectiveAndFutureDate_ThenPriceChangeReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>PC5_MultipleDurationDifferentEffectiveAndFutureDate.JSON</t>
+  </si>
+  <si>
+    <t>PriceChange return 200 ok for valid payload With MultipleDurationDifferentEffectiveAndFutureDate</t>
+  </si>
+  <si>
+    <t>WhenMultipleDurationSameEffectiveDifferentFutureDate_ThenPriceChangeReturn200OkResponse</t>
+  </si>
+  <si>
+    <t>PC6_MultipleDurationSameEffectiveDifferentFutureDate.JSON</t>
+  </si>
+  <si>
+    <t>PriceChange return 200 ok for valid payload With MultipleDurationSameEffectiveDifferentFutureDate</t>
+  </si>
+  <si>
+    <t>WhenPAYSFwith12MonthDuration_PriceChangeAlteredPAYSFPrices</t>
+  </si>
+  <si>
+    <t>PC7_PAYSFDuration12Month.JSON</t>
+  </si>
+  <si>
+    <t>If SAP Price info contains PAYSF with 12 month Duration, PriceChange AltersPAYSF prices in final json</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithOneNewCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithTwoNewCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithOneNewCellScenarioWithourAVCSUoS_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithTwoCellsReplacesOneCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithOneCancelCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWith2CellMetadataChangeScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMetadataChangeScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSimpleUpdateScenarioHavingOneCellWithStatusNameAsUpdate_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSimpleUpdateScenarioHavingOneCellWithStatusNameAsNewEdition_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSimpleUpdateScenarioHavingOneCellStatusNameAsReIssue_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSimpleUpdateScenarioHavingTwoCellsWithDifferentStatusName_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSimpleMoveCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithOneNewCellAndOneMoveOneCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMixScenarioHavingNewCellAndUpdateCellAndMetadataChange_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMixScenarioHavingOneNewCellAndOneCancel&amp;ReplaceCell_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMixScenarioHavingCancel&amp;Replace_UpdateCell_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMixScenarioHavingCancel&amp;ReplaceAndMetadataChangeAndMoveCell_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithNewEditionAdditionalCoverageV01PayloadFile_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithCancelAndReplaceV03PayloadFile_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithCellMoveAndNewCellV03PayloadFile_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithCellMoveV03PayloadFile_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMetadataChangeV03PayloadFile_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMixedScenario1V03PayloadFile_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithNewCellV03PayloadFile_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSupplierDefinedReleasabilitySetV01_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSimpleSuspendedScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSimpleWithdrawnScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithSuspendedAndWithdrawnScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMetadataAndSuspendedMixScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMovedataAndSuspendedMixScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithNewCellScenarioWithMultipleUoSHavingUnitOfSalesTypeUnitButOnly1HavingValueInAddProducts_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithCancel&amp;ReplaceScenarioHavingMultipleUnitOfSalesTypeUnitAndValueInAddProducts_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithCancel&amp;ReplaceWithCancelledCellHaving2UoSButOnly1IsOfTypeUnit_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithMoveAndSuspendedWith2UoSButOnly1HavingValueInAddProduct_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>moveOneCell.JSON</t>
+  </si>
+  <si>
+    <t>oneNewCellAndOneMoveOneCell.JSON</t>
+  </si>
+  <si>
+    <t>newCell_updateCell_metadataChange.JSON</t>
+  </si>
+  <si>
+    <t>newCell_and_CancelReplace.JSON</t>
+  </si>
+  <si>
+    <t>CancelReplace_UpdateCell.JSON</t>
+  </si>
+  <si>
+    <t>CR_metadata_move.JSON</t>
   </si>
 </sst>
 </file>
@@ -563,7 +796,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +812,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -634,14 +873,208 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -943,7 +1376,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1024,15 +1457,15 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C5" s="4" t="str">
         <f t="shared" ref="C5:C33" si="0">CONCATENATE(A5,"_",B5)</f>
@@ -1042,620 +1475,1139 @@
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ID5_1NewCellWoNewAVCSUnit.JSON</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ID5_1NewCellWoNewAVCSUnit.JSON</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ID6_2CellsReplace1CellsCancel.JSON</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ID6_2CellsReplace1CellsCancel.JSON</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="C8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ID7_1CellCancel.JSON</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="E8" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ID7_1CellCancel.JSON</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="C9" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>ID8_2CellMetadataChange.JSON</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>ID8_2CellMetadataChange.JSON</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="C10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ID9_MetadataChange.JSON</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>31</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ID10_UpdateSimple.JSON</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>37</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ID11_updateOneCellWithNewEditionStatus.JSON</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>41</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ID12_updateOneCellWithReIssueStatus.JSON</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>ID13_updateTwoCellsWithDifferentStatusName.JSON</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>50</v>
+        <v>210</v>
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>ID14_ID14_moveOneCell.JSON</v>
+        <v>ID14_moveOneCell.JSON</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>51</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>53</v>
+        <v>211</v>
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>ID15_ID15_oneNewCellAndOneMoveOneCell.JSON</v>
+        <v>ID15_oneNewCellAndOneMoveOneCell.JSON</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>55</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>ID16_ID16_newCell_updateCell_metadataChange.JSON</v>
+        <v>ID16_newCell_updateCell_metadataChange.JSON</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>59</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>61</v>
+        <v>213</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>ID17_ID17_newCell_and_CancelReplace.JSON</v>
+        <v>ID17_newCell_and_CancelReplace.JSON</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>62</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>ID18_ID18_CancelReplace_UpdateCell.JSON</v>
+        <v>ID18_CancelReplace_UpdateCell.JSON</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>118</v>
+        <v>89</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>65</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>67</v>
+        <v>215</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>ID19_ID19_CR_metadata_move.JSON</v>
+        <v>ID19_CR_metadata_move.JSON</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>68</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C21" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID20_New Edition additional coverage v0.1</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>104</v>
+        <v>87</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C22" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID21_cancelAndReplaceV03</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>103</v>
+        <v>22</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C23" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID22_Cell_Moves_Unit_and_New_CellV03</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>102</v>
+        <v>86</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID23_Cell_MoveV03</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>ID23_Cell_MoveV03</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C25" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID24_Metadata_ChangeV03</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>100</v>
+        <v>84</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="C26" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID25_Mixed_scenario1V03</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>105</v>
+        <v>83</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="C27" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID26_New_CellV03</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>99</v>
+        <v>82</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="C28" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID27_supplier_Defined_ReleasabilitySet_V01</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>99</v>
+        <v>81</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="C29" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID28_simpleSuspendedScenario</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>97</v>
+        <v>80</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="C30" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID29_simpleWithdrawnScenario</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C31" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID30_Suspend_and_WithdrawV01</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>96</v>
+        <v>78</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C32" s="5" t="str">
         <f t="shared" si="0"/>
         <v>ID31_metadataAndSuspended</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>95</v>
+        <v>77</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>ID32_moveAndSuspended</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="C33" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>ID32_moveAndSuspended</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="C34" s="5" t="str">
         <f t="shared" ref="C34:C37" si="1">CONCATENATE(A34,"_",B34)</f>
         <v>ID33_NewCell_With2UoS_But_only1_having_addProduct</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>130</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C35" s="5" t="str">
         <f t="shared" si="1"/>
         <v>ID34_Cancel&amp;Replace_With_NewCells_having_2UoS_With_addProductValue</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>129</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C36" s="5" t="str">
         <f t="shared" si="1"/>
         <v>ID35_Cancel&amp;Replace_With_CancelCell_having_2UoS_but_onlyOneAsTypeUnit</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>128</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="C37" s="5" t="str">
         <f t="shared" si="1"/>
         <v>ID36_MoveAndSuspended_With_2UoS_But1_Having_addProductsValue</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>127</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="C38" s="5" t="str">
         <f t="shared" ref="C38" si="2">CONCATENATE(A38,"_",B38)</f>
         <v>ID37_CreateUoSHavingMultipleItemsInAddProducts</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:E37">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:C38 E38">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="25" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="68.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="40" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.5703125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="68.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:D3 B4:B17">
+    <cfRule type="expression" dxfId="24" priority="16">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5 C5:D5">
+    <cfRule type="expression" dxfId="23" priority="15">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7">
+    <cfRule type="expression" dxfId="22" priority="14">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="expression" dxfId="21" priority="13">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="20" priority="12">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A11">
+    <cfRule type="expression" dxfId="19" priority="11">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="expression" dxfId="18" priority="10">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
+    <cfRule type="expression" dxfId="17" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="expression" dxfId="16" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="expression" dxfId="15" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D6">
+    <cfRule type="expression" dxfId="14" priority="6">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:C9">
+    <cfRule type="expression" dxfId="13" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="expression" dxfId="12" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D8">
+    <cfRule type="expression" dxfId="11" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D17">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:C5">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:C3">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:C7">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:C9">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated template along with update in config
</commit_message>
<xml_diff>
--- a/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
+++ b/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prash1501461\Source\Repos\UKHO\erp-facade\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UpdatedERP\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Webhook Scenario Mapping" sheetId="1" r:id="rId1"/>
-    <sheet name="UnitOfSale Scenario mapping" sheetId="2" r:id="rId2"/>
-    <sheet name="PriceChange Scenario Mapping" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="160">
   <si>
     <t>ID#</t>
   </si>
@@ -434,219 +432,6 @@
     <t>WhenICallTheWebhookWithMoveAndNewCellScenarioWhereUoSHasMultipleValuesInAddProducts_ThenWebhookReturns200Response</t>
   </si>
   <si>
-    <t>Webhook Input File name</t>
-  </si>
-  <si>
-    <t>UoS input File name</t>
-  </si>
-  <si>
-    <t>WhenValidEventReceivedWithValidToken_ThenUoSReturns200OkResponse</t>
-  </si>
-  <si>
-    <t>ID1_WebhookPayload.JSON</t>
-  </si>
-  <si>
-    <t>UoS1_Pricing.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and token</t>
-  </si>
-  <si>
-    <t>WhenValidEventReceivedWithInvalidToken_ThenUoSReturns401UnAuthorizedResponse</t>
-  </si>
-  <si>
-    <t>UoS return 401 Unauthorized for valid payload and Invalid token</t>
-  </si>
-  <si>
-    <t>WhenReceivePriceInfoForAllUoSSentToSAP_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>When Receive PriceInfo for All UoS Sent To SAP UoS Return 200Ok Response</t>
-  </si>
-  <si>
-    <t>WhenPriceInfoIsBlankFromSAP_ThenPriceSectionIsEmptyInFinalUoS_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS3_ProductMissingUOS.JSON</t>
-  </si>
-  <si>
-    <t>When PriceInfo is blank from SAP for any product then Price Section Is Empty In Final UoS</t>
-  </si>
-  <si>
-    <t>WhenPriceInfoIsNullFromSAP_ThenPriceSectionIsEmptyInFinalUoS_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS2_ProductISNullUOS.JSON</t>
-  </si>
-  <si>
-    <t>When PriceInfo is null from SAP for any product then Price Section Is Empty In Final UoS</t>
-  </si>
-  <si>
-    <t>WhenNoCorrIdinUoSrequest_UoSReturn400BadrequestResponse</t>
-  </si>
-  <si>
-    <t>When No CorrId in UoSrequest UoS Return 400Badrequest Response</t>
-  </si>
-  <si>
-    <t>WhenInvalidCorrIdinUoSrequest_UoSReturn404NotFoundResponse</t>
-  </si>
-  <si>
-    <t>When Invalid CorrId in UoSrequest UoS Return 400Badrequest Response</t>
-  </si>
-  <si>
-    <t>WhenValidCorrIdPassed_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and shared key</t>
-  </si>
-  <si>
-    <t>WhenValidCorrIdWithFutureDateBlank_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_4_FutureDateFieldBlank.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and Future Date Blank</t>
-  </si>
-  <si>
-    <t>WhenValidCorrIdMultiProdSameDuration_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_5_MultiProductSameDuration.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and same duration for multiple products</t>
-  </si>
-  <si>
-    <t>WhenValidCorrIdMultiProdMultiDuration_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_6_MultiProductMultiDuration.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and multiple duration for multiple products</t>
-  </si>
-  <si>
-    <t>WhenSameEffectiveAndFutureDate_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_7_SameEffectiveSameFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and same Effective and Future Date</t>
-  </si>
-  <si>
-    <t>WhenDiffEffectiveAndSameFutureDate_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_8_DiffEffectiveSameFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and diffrent Effective and same Future Date</t>
-  </si>
-  <si>
-    <t>WhenSameEffectiveAndDiffFutureDate_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_9_SameEffectiveDiffFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and same Effective and different Future Date</t>
-  </si>
-  <si>
-    <t>WhenDiffEffectiveAndDiffFutureDate_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_10_DiffntEffectiveAndDiffFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>WhenPAYSFwith12MonthDuration_UoSAlteredPAYSFPricesFinalJson</t>
-  </si>
-  <si>
-    <t>UoS_12_SAPPricing_PAYSF12Months.JSON</t>
-  </si>
-  <si>
-    <t>If SAP Price info contains PAYSF with 12 month Duration, UoS AltersPAYSF prices in final json</t>
-  </si>
-  <si>
-    <t>PriceChange Input File name</t>
-  </si>
-  <si>
-    <t>WhenValidPriceChangeEventReceivedWithValidToken_ThenPriceChangeReturns200OkResponse</t>
-  </si>
-  <si>
-    <t>PC1_MultipleProduct.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload and token</t>
-  </si>
-  <si>
-    <t>WhenValidPriceChangeEventReceivedWithInvalidToken_ThenPriceChangeReturns401UnAuthorizedResponse</t>
-  </si>
-  <si>
-    <t>PriceChange return 401 Unauthorized for valid payload and Invalid token</t>
-  </si>
-  <si>
-    <t>WhenMultipleProduct_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload and multiple products</t>
-  </si>
-  <si>
-    <t>WhenFutureDateBlank_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC2_FutureDateBlank.JSON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PriceChange return 200 ok for valid payload and FutureDate Field as Blank </t>
-  </si>
-  <si>
-    <t>WhenMultipleProductDifferentDuration_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC3_MultipleProductDifferentDuration.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload With MultipleProductDifferentDuration</t>
-  </si>
-  <si>
-    <t>WhenMultipleDurationSameEffectiveAndFutureDate_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC4_MultipleDurationSameEffectiveAndFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload With MultipleDurationSameEffectiveAndFutureDate</t>
-  </si>
-  <si>
-    <t>WhenMultipleDurationDifferentEffectiveAndFutureDate_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC5_MultipleDurationDifferentEffectiveAndFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload With MultipleDurationDifferentEffectiveAndFutureDate</t>
-  </si>
-  <si>
-    <t>WhenMultipleDurationSameEffectiveDifferentFutureDate_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC6_MultipleDurationSameEffectiveDifferentFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload With MultipleDurationSameEffectiveDifferentFutureDate</t>
-  </si>
-  <si>
-    <t>WhenPAYSFwith12MonthDuration_PriceChangeAlteredPAYSFPrices</t>
-  </si>
-  <si>
-    <t>PC7_PAYSFDuration12Month.JSON</t>
-  </si>
-  <si>
-    <t>If SAP Price info contains PAYSF with 12 month Duration, PriceChange AltersPAYSF prices in final json</t>
-  </si>
-  <si>
     <t>WhenICallTheWebhookWithOneNewCellScenario_ThenWebhookReturns200Response</t>
   </si>
   <si>
@@ -765,6 +550,73 @@
   </si>
   <si>
     <t>CR_metadata_move.JSON</t>
+  </si>
+  <si>
+    <t>ID38_3AdditionalCoverageCell.JSON</t>
+  </si>
+  <si>
+    <t>ID39_1AdditionalCoverageWithReplacedCell.JSON</t>
+  </si>
+  <si>
+    <t>ID40_1AdditionalCoverageWithReplacedCellAnd1CancelledCell.JSON</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithThreeAdditionalCoverageCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithOneAdditionalCoverageWithReplacedCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithOneAdditionalCoverageWithReplacedAndOneCancelledCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>3 Additional Coverage Cell</t>
+  </si>
+  <si>
+    <t>OneAdditionalCoverageWithReplaced</t>
+  </si>
+  <si>
+    <t>OneAdditionalCoverageWithReplacedAndOneCancelledCell</t>
+  </si>
+  <si>
+    <t>Cell1:
+"additionalCoverage": ["DK4LIMFW","DK4LIMUT","DK4LIMNU"] 
+contentChanged = true and isNewCell = false 
+AND
+"statusName": "New Edition"
+"removeProducts": [ "DE416080" ]
+"removeProducts": [ "DE416080" ]</t>
+  </si>
+  <si>
+    <t>Cell1:
+"replacedBy": ["US4AK6NT"]
+ "additionalCoverage": ["DK4LIMFW"]
+contentChanged = true and isNewCell = false 
+AND
+"statusName": "New Edition"
+Cell2:
+contentChanged = true and isNewCell = false 
+AND
+"statusName": "New Edition"</t>
+  </si>
+  <si>
+    <t>ID38</t>
+  </si>
+  <si>
+    <t>ID39</t>
+  </si>
+  <si>
+    <t>Cell1:
+"replacedBy": ["US4AK6NT"]
+ "additionalCoverage": ["DK4LIMFW"]
+"statusName": "Cancellation Update"
+Cell2:
+contentChanged = true and isNewCell = false 
+AND
+"statusName": "New Edition"</t>
+  </si>
+  <si>
+    <t>ID40</t>
   </si>
 </sst>
 </file>
@@ -796,7 +648,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -812,12 +664,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -849,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -873,180 +719,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -1372,24 +1049,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.5703125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.54296875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="45.26953125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="55.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.54296875" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1083,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1424,7 +1101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1442,7 +1119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1457,10 +1134,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1475,10 +1152,10 @@
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1493,10 +1170,10 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1511,10 +1188,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1529,10 +1206,10 @@
         <v>25</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1547,10 +1224,10 @@
         <v>28</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -1565,10 +1242,10 @@
         <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -1583,10 +1260,10 @@
         <v>33</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
@@ -1601,10 +1278,10 @@
         <v>36</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1619,10 +1296,10 @@
         <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1637,15 +1314,15 @@
         <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1655,15 +1332,15 @@
         <v>98</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1673,15 +1350,15 @@
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>212</v>
+        <v>141</v>
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1691,15 +1368,15 @@
         <v>47</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1709,15 +1386,15 @@
         <v>22</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1727,15 +1404,15 @@
         <v>89</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1745,10 +1422,10 @@
         <v>88</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -1763,10 +1440,10 @@
         <v>87</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>52</v>
       </c>
@@ -1781,10 +1458,10 @@
         <v>22</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>53</v>
       </c>
@@ -1799,10 +1476,10 @@
         <v>86</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>54</v>
       </c>
@@ -1817,10 +1494,10 @@
         <v>85</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>55</v>
       </c>
@@ -1835,10 +1512,10 @@
         <v>84</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
@@ -1853,10 +1530,10 @@
         <v>83</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>57</v>
       </c>
@@ -1871,10 +1548,10 @@
         <v>82</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -1889,10 +1566,10 @@
         <v>81</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>59</v>
       </c>
@@ -1907,10 +1584,10 @@
         <v>80</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>60</v>
       </c>
@@ -1925,10 +1602,10 @@
         <v>79</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
@@ -1943,10 +1620,10 @@
         <v>78</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
@@ -1961,10 +1638,10 @@
         <v>77</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>63</v>
       </c>
@@ -1979,10 +1656,10 @@
         <v>99</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>90</v>
       </c>
@@ -1997,10 +1674,10 @@
         <v>100</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
@@ -2015,10 +1692,10 @@
         <v>22</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>92</v>
       </c>
@@ -2033,10 +1710,10 @@
         <v>22</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>93</v>
       </c>
@@ -2051,10 +1728,10 @@
         <v>99</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>101</v>
       </c>
@@ -2072,542 +1749,94 @@
         <v>104</v>
       </c>
     </row>
+    <row r="39" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:E37">
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:C38 E38">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39:E39">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:C40 E40">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:E41">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="68.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40" style="2" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="68.7109375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:D3 B4:B17">
-    <cfRule type="expression" dxfId="24" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5 C5:D5">
-    <cfRule type="expression" dxfId="23" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="22" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="21" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="20" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="19" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="18" priority="10">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="expression" dxfId="17" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="16" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="15" priority="7">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="14" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C9">
-    <cfRule type="expression" dxfId="13" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="12" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="11" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="10" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D17">
-    <cfRule type="expression" dxfId="9" priority="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="63.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:C5">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:C3">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7:C7">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:C9">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
WIP- Feature/add env check for performance test script (#131)
* added env check for one test case

* Moved env check to init section & done code optimization

* 147012 removed eesevents table data from main variable files AB#147012

* 147012- Removed PT script of priceinformation end point as it has been removed as a part of WA CR

* 147012 - Updated Readme.md file as per CR requirement

* 147012- Added appinsight fields AB#147012

* Updated template along with update in config

* Remove Polygons and comment section

* Resolved Review comments

* 147012- Removed appinsight fields AB#147012

* removed SharedKeyConfigurationKey E2E Live IAT

* updated file property

---------

Co-authored-by: Vishal Dukare <Vishal14583@Mastek.Com>
Co-authored-by: Sadha1501493 <sadha1501493@mastek.com>
Co-authored-by: Vinod Nerella <vinod1502506@mastek.com>
Co-authored-by: Sakshi Singhal <sakshi15525@mastek.com>
Co-authored-by: Pradeep I <pradeep15558@mastek.com>
</commit_message>
<xml_diff>
--- a/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
+++ b/tests/UKHO.ERPFacade.API.FunctionalTests/ERPFacadeScenarioData/Scenario Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prash1501461\Source\Repos\UKHO\erp-facade\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UpdatedERP\tests\UKHO.ERPFacade.API.FunctionalTests\ERPFacadeScenarioData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,8 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Webhook Scenario Mapping" sheetId="1" r:id="rId1"/>
-    <sheet name="UnitOfSale Scenario mapping" sheetId="2" r:id="rId2"/>
-    <sheet name="PriceChange Scenario Mapping" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="160">
   <si>
     <t>ID#</t>
   </si>
@@ -434,219 +432,6 @@
     <t>WhenICallTheWebhookWithMoveAndNewCellScenarioWhereUoSHasMultipleValuesInAddProducts_ThenWebhookReturns200Response</t>
   </si>
   <si>
-    <t>Webhook Input File name</t>
-  </si>
-  <si>
-    <t>UoS input File name</t>
-  </si>
-  <si>
-    <t>WhenValidEventReceivedWithValidToken_ThenUoSReturns200OkResponse</t>
-  </si>
-  <si>
-    <t>ID1_WebhookPayload.JSON</t>
-  </si>
-  <si>
-    <t>UoS1_Pricing.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and token</t>
-  </si>
-  <si>
-    <t>WhenValidEventReceivedWithInvalidToken_ThenUoSReturns401UnAuthorizedResponse</t>
-  </si>
-  <si>
-    <t>UoS return 401 Unauthorized for valid payload and Invalid token</t>
-  </si>
-  <si>
-    <t>WhenReceivePriceInfoForAllUoSSentToSAP_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>When Receive PriceInfo for All UoS Sent To SAP UoS Return 200Ok Response</t>
-  </si>
-  <si>
-    <t>WhenPriceInfoIsBlankFromSAP_ThenPriceSectionIsEmptyInFinalUoS_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS3_ProductMissingUOS.JSON</t>
-  </si>
-  <si>
-    <t>When PriceInfo is blank from SAP for any product then Price Section Is Empty In Final UoS</t>
-  </si>
-  <si>
-    <t>WhenPriceInfoIsNullFromSAP_ThenPriceSectionIsEmptyInFinalUoS_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS2_ProductISNullUOS.JSON</t>
-  </si>
-  <si>
-    <t>When PriceInfo is null from SAP for any product then Price Section Is Empty In Final UoS</t>
-  </si>
-  <si>
-    <t>WhenNoCorrIdinUoSrequest_UoSReturn400BadrequestResponse</t>
-  </si>
-  <si>
-    <t>When No CorrId in UoSrequest UoS Return 400Badrequest Response</t>
-  </si>
-  <si>
-    <t>WhenInvalidCorrIdinUoSrequest_UoSReturn404NotFoundResponse</t>
-  </si>
-  <si>
-    <t>When Invalid CorrId in UoSrequest UoS Return 400Badrequest Response</t>
-  </si>
-  <si>
-    <t>WhenValidCorrIdPassed_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and shared key</t>
-  </si>
-  <si>
-    <t>WhenValidCorrIdWithFutureDateBlank_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_4_FutureDateFieldBlank.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and Future Date Blank</t>
-  </si>
-  <si>
-    <t>WhenValidCorrIdMultiProdSameDuration_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_5_MultiProductSameDuration.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and same duration for multiple products</t>
-  </si>
-  <si>
-    <t>WhenValidCorrIdMultiProdMultiDuration_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_6_MultiProductMultiDuration.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and multiple duration for multiple products</t>
-  </si>
-  <si>
-    <t>WhenSameEffectiveAndFutureDate_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_7_SameEffectiveSameFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and same Effective and Future Date</t>
-  </si>
-  <si>
-    <t>WhenDiffEffectiveAndSameFutureDate_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_8_DiffEffectiveSameFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and diffrent Effective and same Future Date</t>
-  </si>
-  <si>
-    <t>WhenSameEffectiveAndDiffFutureDate_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_9_SameEffectiveDiffFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>UoS return 200 ok for valid payload and same Effective and different Future Date</t>
-  </si>
-  <si>
-    <t>WhenDiffEffectiveAndDiffFutureDate_UoSReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>UoS_10_DiffntEffectiveAndDiffFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>WhenPAYSFwith12MonthDuration_UoSAlteredPAYSFPricesFinalJson</t>
-  </si>
-  <si>
-    <t>UoS_12_SAPPricing_PAYSF12Months.JSON</t>
-  </si>
-  <si>
-    <t>If SAP Price info contains PAYSF with 12 month Duration, UoS AltersPAYSF prices in final json</t>
-  </si>
-  <si>
-    <t>PriceChange Input File name</t>
-  </si>
-  <si>
-    <t>WhenValidPriceChangeEventReceivedWithValidToken_ThenPriceChangeReturns200OkResponse</t>
-  </si>
-  <si>
-    <t>PC1_MultipleProduct.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload and token</t>
-  </si>
-  <si>
-    <t>WhenValidPriceChangeEventReceivedWithInvalidToken_ThenPriceChangeReturns401UnAuthorizedResponse</t>
-  </si>
-  <si>
-    <t>PriceChange return 401 Unauthorized for valid payload and Invalid token</t>
-  </si>
-  <si>
-    <t>WhenMultipleProduct_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload and multiple products</t>
-  </si>
-  <si>
-    <t>WhenFutureDateBlank_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC2_FutureDateBlank.JSON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PriceChange return 200 ok for valid payload and FutureDate Field as Blank </t>
-  </si>
-  <si>
-    <t>WhenMultipleProductDifferentDuration_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC3_MultipleProductDifferentDuration.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload With MultipleProductDifferentDuration</t>
-  </si>
-  <si>
-    <t>WhenMultipleDurationSameEffectiveAndFutureDate_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC4_MultipleDurationSameEffectiveAndFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload With MultipleDurationSameEffectiveAndFutureDate</t>
-  </si>
-  <si>
-    <t>WhenMultipleDurationDifferentEffectiveAndFutureDate_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC5_MultipleDurationDifferentEffectiveAndFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload With MultipleDurationDifferentEffectiveAndFutureDate</t>
-  </si>
-  <si>
-    <t>WhenMultipleDurationSameEffectiveDifferentFutureDate_ThenPriceChangeReturn200OkResponse</t>
-  </si>
-  <si>
-    <t>PC6_MultipleDurationSameEffectiveDifferentFutureDate.JSON</t>
-  </si>
-  <si>
-    <t>PriceChange return 200 ok for valid payload With MultipleDurationSameEffectiveDifferentFutureDate</t>
-  </si>
-  <si>
-    <t>WhenPAYSFwith12MonthDuration_PriceChangeAlteredPAYSFPrices</t>
-  </si>
-  <si>
-    <t>PC7_PAYSFDuration12Month.JSON</t>
-  </si>
-  <si>
-    <t>If SAP Price info contains PAYSF with 12 month Duration, PriceChange AltersPAYSF prices in final json</t>
-  </si>
-  <si>
     <t>WhenICallTheWebhookWithOneNewCellScenario_ThenWebhookReturns200Response</t>
   </si>
   <si>
@@ -765,6 +550,70 @@
   </si>
   <si>
     <t>CR_metadata_move.JSON</t>
+  </si>
+  <si>
+    <t>ID38_3AdditionalCoverageCell.JSON</t>
+  </si>
+  <si>
+    <t>ID40_1AdditionalCoverageWithReplacedCellAnd1CancelledCell.JSON</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithThreeAdditionalCoverageCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithOneAdditionalCoverageWithReplacedAndOneCancelledCellScenario_ThenWebhookReturns200Response</t>
+  </si>
+  <si>
+    <t>3 Additional Coverage Cell</t>
+  </si>
+  <si>
+    <t>OneAdditionalCoverageWithReplaced</t>
+  </si>
+  <si>
+    <t>OneAdditionalCoverageWithReplacedAndOneCancelledCell</t>
+  </si>
+  <si>
+    <t>ID38</t>
+  </si>
+  <si>
+    <t>ID39</t>
+  </si>
+  <si>
+    <t>ID40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHEN EXIST multiple additionalCoverage AND
+WHEN EXIST removeProduct item AND
+isNewCell = true &amp; IsNewUnitOfSale = true
+WHEN StatusName = “New Edition” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell 1
+WHEN EXIST additionalCoverage AND
+WHEN StatusName = “Cancellation Update” AND
+contentChanged = true and isNewCell = false AND
+WHEN StatusName = “New Edition” 
+Cell2:
+contentChanged = true and isNewCell = false 
+AND
+WHEN StatusName = "New Edition"
+</t>
+  </si>
+  <si>
+    <t>Cell 1
+WHEN EXIST additionalCoverage AND
+WHEN EXIST replacedBy items AND
+WHEN StatusName = “Cancellation Update” AND
+Cell2:
+contentChanged = true and isNewCell = false 
+AND
+WHEN StatusName = "New Edition"</t>
+  </si>
+  <si>
+    <t>ID39_1AdditionalCoverageWith1CancelledCell.JSON</t>
+  </si>
+  <si>
+    <t>WhenICallTheWebhookWithOneAdditionalCoverageWithCancelledCellScenario_ThenWebhookReturns200Response</t>
   </si>
 </sst>
 </file>
@@ -796,7 +645,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -812,12 +661,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -849,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -873,180 +716,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -1372,24 +1046,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="44.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="45.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="54.5703125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.54296875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="44.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="45.26953125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="55.7265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.54296875" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1424,7 +1098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1442,7 +1116,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -1457,10 +1131,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1475,10 +1149,10 @@
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1493,10 +1167,10 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1511,10 +1185,10 @@
         <v>22</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1529,10 +1203,10 @@
         <v>25</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -1547,10 +1221,10 @@
         <v>28</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -1565,10 +1239,10 @@
         <v>28</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -1583,10 +1257,10 @@
         <v>33</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>34</v>
       </c>
@@ -1601,10 +1275,10 @@
         <v>36</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1619,10 +1293,10 @@
         <v>39</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
@@ -1637,15 +1311,15 @@
         <v>42</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>210</v>
+        <v>139</v>
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1655,15 +1329,15 @@
         <v>98</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1673,15 +1347,15 @@
         <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>212</v>
+        <v>141</v>
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1691,15 +1365,15 @@
         <v>47</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1709,15 +1383,15 @@
         <v>22</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1727,15 +1401,15 @@
         <v>89</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1745,10 +1419,10 @@
         <v>88</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
@@ -1763,10 +1437,10 @@
         <v>87</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>52</v>
       </c>
@@ -1781,10 +1455,10 @@
         <v>22</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>53</v>
       </c>
@@ -1799,10 +1473,10 @@
         <v>86</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>54</v>
       </c>
@@ -1817,10 +1491,10 @@
         <v>85</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>55</v>
       </c>
@@ -1835,10 +1509,10 @@
         <v>84</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>56</v>
       </c>
@@ -1853,10 +1527,10 @@
         <v>83</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>57</v>
       </c>
@@ -1871,10 +1545,10 @@
         <v>82</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -1889,10 +1563,10 @@
         <v>81</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>59</v>
       </c>
@@ -1907,10 +1581,10 @@
         <v>80</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>60</v>
       </c>
@@ -1925,10 +1599,10 @@
         <v>79</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>61</v>
       </c>
@@ -1943,10 +1617,10 @@
         <v>78</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
@@ -1961,10 +1635,10 @@
         <v>77</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>63</v>
       </c>
@@ -1979,10 +1653,10 @@
         <v>99</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>90</v>
       </c>
@@ -1997,10 +1671,10 @@
         <v>100</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
@@ -2015,10 +1689,10 @@
         <v>22</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>92</v>
       </c>
@@ -2033,10 +1707,10 @@
         <v>22</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>93</v>
       </c>
@@ -2051,10 +1725,10 @@
         <v>99</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>101</v>
       </c>
@@ -2072,542 +1746,94 @@
         <v>104</v>
       </c>
     </row>
+    <row r="39" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A40" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:E37">
-    <cfRule type="expression" dxfId="27" priority="3">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:C38 E38">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="25" priority="1">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39:E39">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:C40 E40">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41:E41">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="68.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40" style="2" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="68.7109375" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:D3 B4:B17">
-    <cfRule type="expression" dxfId="24" priority="16">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5 C5:D5">
-    <cfRule type="expression" dxfId="23" priority="15">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7">
-    <cfRule type="expression" dxfId="22" priority="14">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9">
-    <cfRule type="expression" dxfId="21" priority="13">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="20" priority="12">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A11">
-    <cfRule type="expression" dxfId="19" priority="11">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="18" priority="10">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
-    <cfRule type="expression" dxfId="17" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="16" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A15">
-    <cfRule type="expression" dxfId="15" priority="7">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="14" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:C9">
-    <cfRule type="expression" dxfId="13" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="12" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="11" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="10" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D17">
-    <cfRule type="expression" dxfId="9" priority="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="63.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="52.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:C5">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:C3">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7:C7">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:C9">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>